<commit_message>
added structural parameters as option in runsim
</commit_message>
<xml_diff>
--- a/Paper_new/Model/sim_results.xlsx
+++ b/Paper_new/Model/sim_results.xlsx
@@ -16,6 +16,7 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="SWOPIT_NONE_ALL_250" sheetId="2" r:id="rId4"/>
     <sheet name="SWOPIT_NONE_TRUE_STRAT_250" sheetId="3" r:id="rId6"/>
+    <sheet name="SWOPIT_NONE_TRUE_250" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029" fullCalcOnLoad="true"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="214">
   <si>
     <t>ESTIMATION RESULTS for SWOPIT_NONE_ALL_250</t>
   </si>
@@ -233,6 +234,450 @@
   </si>
   <si>
     <t>MARGINAL EFFECT SWOPIT_NONE_TRUE_STRAT_250</t>
+  </si>
+  <si>
+    <t>ESTIMATION RESULTS for SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Mins</t>
+  </si>
+  <si>
+    <t>Secs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converged: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Converged: </t>
+  </si>
+  <si>
+    <t>Startiter:</t>
+  </si>
+  <si>
+    <t>Runtime:</t>
+  </si>
+  <si>
+    <t>PARAMETERS SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>NAMES</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean ci_low</t>
+  </si>
+  <si>
+    <t>mean ci_high</t>
+  </si>
+  <si>
+    <t>mean se</t>
+  </si>
+  <si>
+    <t>real se</t>
+  </si>
+  <si>
+    <t>real2mean se</t>
+  </si>
+  <si>
+    <t>real2median se</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>reg_cutoff</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>out1_cutoff1</t>
+  </si>
+  <si>
+    <t>out1_cutoff2</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>out2_cutoff1</t>
+  </si>
+  <si>
+    <t>out2_cutoff2</t>
+  </si>
+  <si>
+    <t>PROBABILITIES SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>Choice/Reg</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean ci_low</t>
+  </si>
+  <si>
+    <t>mean ci_high</t>
+  </si>
+  <si>
+    <t>mean se</t>
+  </si>
+  <si>
+    <t>real se</t>
+  </si>
+  <si>
+    <t>real2mean se</t>
+  </si>
+  <si>
+    <t>real2median se</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>Choice 1</t>
+  </si>
+  <si>
+    <t>Choice 2</t>
+  </si>
+  <si>
+    <t>Choice 3</t>
+  </si>
+  <si>
+    <t>Reg 1</t>
+  </si>
+  <si>
+    <t>Reg 2</t>
+  </si>
+  <si>
+    <t>MARGINAL EFFECT SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>NAMES</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean ci_low</t>
+  </si>
+  <si>
+    <t>mean ci_high</t>
+  </si>
+  <si>
+    <t>mean se</t>
+  </si>
+  <si>
+    <t>real se</t>
+  </si>
+  <si>
+    <t>real2mean se</t>
+  </si>
+  <si>
+    <t>real2median se</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>X1 on 1</t>
+  </si>
+  <si>
+    <t>X1 on 2</t>
+  </si>
+  <si>
+    <t>X1 on 3</t>
+  </si>
+  <si>
+    <t>X2 on 1</t>
+  </si>
+  <si>
+    <t>X2 on 2</t>
+  </si>
+  <si>
+    <t>X2 on 3</t>
+  </si>
+  <si>
+    <t>X3 on 1</t>
+  </si>
+  <si>
+    <t>X3 on 2</t>
+  </si>
+  <si>
+    <t>X3 on 3</t>
+  </si>
+  <si>
+    <t>X4 on 1</t>
+  </si>
+  <si>
+    <t>X4 on 2</t>
+  </si>
+  <si>
+    <t>X4 on 3</t>
+  </si>
+  <si>
+    <t>X5 on 1</t>
+  </si>
+  <si>
+    <t>X5 on 2</t>
+  </si>
+  <si>
+    <t>X5 on 3</t>
+  </si>
+  <si>
+    <t>ESTIMATION RESULTS for SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Mins</t>
+  </si>
+  <si>
+    <t>Secs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converged: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not Converged: </t>
+  </si>
+  <si>
+    <t>Startiter:</t>
+  </si>
+  <si>
+    <t>Runtime:</t>
+  </si>
+  <si>
+    <t>PARAMETERS SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>NAMES</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean ci_low</t>
+  </si>
+  <si>
+    <t>mean ci_high</t>
+  </si>
+  <si>
+    <t>mean se</t>
+  </si>
+  <si>
+    <t>real se</t>
+  </si>
+  <si>
+    <t>real2mean se</t>
+  </si>
+  <si>
+    <t>real2median se</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>reg_cutoff</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>out1_cutoff1</t>
+  </si>
+  <si>
+    <t>out1_cutoff2</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b5</t>
+  </si>
+  <si>
+    <t>out2_cutoff1</t>
+  </si>
+  <si>
+    <t>out2_cutoff2</t>
+  </si>
+  <si>
+    <t>PROBABILITIES SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>Choice/Reg</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean ci_low</t>
+  </si>
+  <si>
+    <t>mean ci_high</t>
+  </si>
+  <si>
+    <t>mean se</t>
+  </si>
+  <si>
+    <t>real se</t>
+  </si>
+  <si>
+    <t>real2mean se</t>
+  </si>
+  <si>
+    <t>real2median se</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>Choice 1</t>
+  </si>
+  <si>
+    <t>Choice 2</t>
+  </si>
+  <si>
+    <t>Choice 3</t>
+  </si>
+  <si>
+    <t>Reg 1</t>
+  </si>
+  <si>
+    <t>Reg 2</t>
+  </si>
+  <si>
+    <t>MARGINAL EFFECT SWOPIT_NONE_TRUE_250</t>
+  </si>
+  <si>
+    <t>NAMES</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean ci_low</t>
+  </si>
+  <si>
+    <t>mean ci_high</t>
+  </si>
+  <si>
+    <t>mean se</t>
+  </si>
+  <si>
+    <t>real se</t>
+  </si>
+  <si>
+    <t>real2mean se</t>
+  </si>
+  <si>
+    <t>real2median se</t>
+  </si>
+  <si>
+    <t>rmse</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>X1 on 1</t>
+  </si>
+  <si>
+    <t>X1 on 2</t>
+  </si>
+  <si>
+    <t>X1 on 3</t>
+  </si>
+  <si>
+    <t>X2 on 1</t>
+  </si>
+  <si>
+    <t>X2 on 2</t>
+  </si>
+  <si>
+    <t>X2 on 3</t>
+  </si>
+  <si>
+    <t>X3 on 1</t>
+  </si>
+  <si>
+    <t>X3 on 2</t>
+  </si>
+  <si>
+    <t>X3 on 3</t>
+  </si>
+  <si>
+    <t>X4 on 1</t>
+  </si>
+  <si>
+    <t>X4 on 2</t>
+  </si>
+  <si>
+    <t>X4 on 3</t>
+  </si>
+  <si>
+    <t>X5 on 1</t>
+  </si>
+  <si>
+    <t>X5 on 2</t>
+  </si>
+  <si>
+    <t>X5 on 3</t>
   </si>
 </sst>
 </file>
@@ -3792,4 +4237,1231 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K43"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F3" s="0">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" s="0">
+        <v>0</v>
+      </c>
+      <c r="J3" s="0">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" t="s">
+        <v>158</v>
+      </c>
+      <c r="K5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="0">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0">
+        <v>2.308942002382028</v>
+      </c>
+      <c r="D6" s="0">
+        <v>1.0296123777843826</v>
+      </c>
+      <c r="E6" s="0">
+        <v>3.5882716269796733</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.65273119031208449</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0.19685624139616253</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0.3015885318764091</v>
+      </c>
+      <c r="I6" s="0">
+        <v>0.3015885318764091</v>
+      </c>
+      <c r="J6" s="0">
+        <v>0.36632982490160582</v>
+      </c>
+      <c r="K6" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="0">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="C7" s="0">
+        <v>-0.023488126569383788</v>
+      </c>
+      <c r="D7" s="0">
+        <v>-0.60106948767062574</v>
+      </c>
+      <c r="E7" s="0">
+        <v>0.55409323453185833</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.29468978290271164</v>
+      </c>
+      <c r="G7" s="0">
+        <v>0.027866256961893661</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0.09456132712647651</v>
+      </c>
+      <c r="I7" s="0">
+        <v>0.09456132712647651</v>
+      </c>
+      <c r="J7" s="0">
+        <v>0.22521871812653407</v>
+      </c>
+      <c r="K7" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="0">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0">
+        <v>2.1204793560804007</v>
+      </c>
+      <c r="D8" s="0">
+        <v>1.098956938519267</v>
+      </c>
+      <c r="E8" s="0">
+        <v>3.1420017736415344</v>
+      </c>
+      <c r="F8" s="0">
+        <v>0.52119448398989587</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0.13485424150793313</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0.25874073047662466</v>
+      </c>
+      <c r="I8" s="0">
+        <v>0.25874073047662466</v>
+      </c>
+      <c r="J8" s="0">
+        <v>0.18083401697199541</v>
+      </c>
+      <c r="K8" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="0">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0.99430707012951403</v>
+      </c>
+      <c r="D9" s="0">
+        <v>0.47123197774861564</v>
+      </c>
+      <c r="E9" s="0">
+        <v>1.5173821625104127</v>
+      </c>
+      <c r="F9" s="0">
+        <v>0.26687995111484097</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0.039671795032221784</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0.14865033835063404</v>
+      </c>
+      <c r="I9" s="0">
+        <v>0.14865033835063404</v>
+      </c>
+      <c r="J9" s="0">
+        <v>0.040078183237129</v>
+      </c>
+      <c r="K9" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>164</v>
+      </c>
+      <c r="B10" s="0">
+        <v>-3.8300000000000001</v>
+      </c>
+      <c r="C10" s="0">
+        <v>-3.8014574741731479</v>
+      </c>
+      <c r="D10" s="0">
+        <v>-5.8196150135731299</v>
+      </c>
+      <c r="E10" s="0">
+        <v>-1.7832999347731666</v>
+      </c>
+      <c r="F10" s="0">
+        <v>1.0296911347958184</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0.11068148337835182</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0.10748998378071818</v>
+      </c>
+      <c r="I10" s="0">
+        <v>0.10748998378071818</v>
+      </c>
+      <c r="J10" s="0">
+        <v>0.11430252203433167</v>
+      </c>
+      <c r="K10" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="0">
+        <v>3.7599999999999998</v>
+      </c>
+      <c r="C11" s="0">
+        <v>3.957347871891117</v>
+      </c>
+      <c r="D11" s="0">
+        <v>1.9065762250737548</v>
+      </c>
+      <c r="E11" s="0">
+        <v>6.0081195187084786</v>
+      </c>
+      <c r="F11" s="0">
+        <v>1.0463312912857521</v>
+      </c>
+      <c r="G11" s="0">
+        <v>0.30405860814442259</v>
+      </c>
+      <c r="H11" s="0">
+        <v>0.29059496803425378</v>
+      </c>
+      <c r="I11" s="0">
+        <v>0.29059496803425378</v>
+      </c>
+      <c r="J11" s="0">
+        <v>0.36248837185029292</v>
+      </c>
+      <c r="K11" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="0">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0">
+        <v>1.2972650094676323</v>
+      </c>
+      <c r="D12" s="0">
+        <v>0.54349234713706063</v>
+      </c>
+      <c r="E12" s="0">
+        <v>2.0510376717982037</v>
+      </c>
+      <c r="F12" s="0">
+        <v>0.38458495578298091</v>
+      </c>
+      <c r="G12" s="0">
+        <v>0.26412664696620752</v>
+      </c>
+      <c r="H12" s="0">
+        <v>0.6867836169734437</v>
+      </c>
+      <c r="I12" s="0">
+        <v>0.6867836169734437</v>
+      </c>
+      <c r="J12" s="0">
+        <v>0.39765483964287807</v>
+      </c>
+      <c r="K12" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="0">
+        <v>-2</v>
+      </c>
+      <c r="C13" s="0">
+        <v>-2.4891349731677042</v>
+      </c>
+      <c r="D13" s="0">
+        <v>-3.8915905586309063</v>
+      </c>
+      <c r="E13" s="0">
+        <v>-1.086679387704502</v>
+      </c>
+      <c r="F13" s="0">
+        <v>0.71555171244246996</v>
+      </c>
+      <c r="G13" s="0">
+        <v>0.35592377481144943</v>
+      </c>
+      <c r="H13" s="0">
+        <v>0.49741167356938659</v>
+      </c>
+      <c r="I13" s="0">
+        <v>0.49741167356938659</v>
+      </c>
+      <c r="J13" s="0">
+        <v>0.60492541313107517</v>
+      </c>
+      <c r="K13" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="0">
+        <v>-3.9700000000000002</v>
+      </c>
+      <c r="C14" s="0">
+        <v>-5.0050694401860794</v>
+      </c>
+      <c r="D14" s="0">
+        <v>-7.792360258666827</v>
+      </c>
+      <c r="E14" s="0">
+        <v>-2.2177786217053326</v>
+      </c>
+      <c r="F14" s="0">
+        <v>1.4221132839514103</v>
+      </c>
+      <c r="G14" s="0">
+        <v>0.86565680706225656</v>
+      </c>
+      <c r="H14" s="0">
+        <v>0.60871156808055926</v>
+      </c>
+      <c r="I14" s="0">
+        <v>0.60871156808055926</v>
+      </c>
+      <c r="J14" s="0">
+        <v>1.3493444532884642</v>
+      </c>
+      <c r="K14" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>169</v>
+      </c>
+      <c r="B15" s="0">
+        <v>3.9700000000000002</v>
+      </c>
+      <c r="C15" s="0">
+        <v>4.8973168503969733</v>
+      </c>
+      <c r="D15" s="0">
+        <v>2.000185461677221</v>
+      </c>
+      <c r="E15" s="0">
+        <v>7.7944482391167256</v>
+      </c>
+      <c r="F15" s="0">
+        <v>1.4781554210036285</v>
+      </c>
+      <c r="G15" s="0">
+        <v>0.88345568745685199</v>
+      </c>
+      <c r="H15" s="0">
+        <v>0.59767442239396507</v>
+      </c>
+      <c r="I15" s="0">
+        <v>0.59767442239396507</v>
+      </c>
+      <c r="J15" s="0">
+        <v>1.2807851079435695</v>
+      </c>
+      <c r="K15" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E19" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19" t="s">
+        <v>179</v>
+      </c>
+      <c r="J19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K19" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0.34081173787569552</v>
+      </c>
+      <c r="C20" s="0">
+        <v>0.42155510504461091</v>
+      </c>
+      <c r="D20" s="0">
+        <v>0.16425103686925702</v>
+      </c>
+      <c r="E20" s="0">
+        <v>0.67885917321996481</v>
+      </c>
+      <c r="F20" s="0">
+        <v>0.13127999810452418</v>
+      </c>
+      <c r="G20" s="0">
+        <v>0.019674932229182509</v>
+      </c>
+      <c r="H20" s="0">
+        <v>0.14986999172194893</v>
+      </c>
+      <c r="I20" s="0">
+        <v>0.14986999172194893</v>
+      </c>
+      <c r="J20" s="0">
+        <v>0.084628847363468498</v>
+      </c>
+      <c r="K20" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0.33322877508788151</v>
+      </c>
+      <c r="C21" s="0">
+        <v>0.4273943182615455</v>
+      </c>
+      <c r="D21" s="0">
+        <v>0.1097162034830334</v>
+      </c>
+      <c r="E21" s="0">
+        <v>0.74507243304005766</v>
+      </c>
+      <c r="F21" s="0">
+        <v>0.1620836491304517</v>
+      </c>
+      <c r="G21" s="0">
+        <v>0.0094599176904864267</v>
+      </c>
+      <c r="H21" s="0">
+        <v>0.058364417023167393</v>
+      </c>
+      <c r="I21" s="0">
+        <v>0.058364417023167393</v>
+      </c>
+      <c r="J21" s="0">
+        <v>0.10008465497157898</v>
+      </c>
+      <c r="K21" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0.32595948703642297</v>
+      </c>
+      <c r="C22" s="0">
+        <v>0.15105057669384356</v>
+      </c>
+      <c r="D22" s="0">
+        <v>-0.092303511215936523</v>
+      </c>
+      <c r="E22" s="0">
+        <v>0.39440466460362367</v>
+      </c>
+      <c r="F22" s="0">
+        <v>0.12416253044919506</v>
+      </c>
+      <c r="G22" s="0">
+        <v>0.0016668143207748958</v>
+      </c>
+      <c r="H22" s="0">
+        <v>0.013424455145563615</v>
+      </c>
+      <c r="I22" s="0">
+        <v>0.013424455145563615</v>
+      </c>
+      <c r="J22" s="0">
+        <v>0.18467412462890859</v>
+      </c>
+      <c r="K22" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="0">
+        <v>0.49139299470263359</v>
+      </c>
+      <c r="C23" s="0">
+        <v>0.39014271432940251</v>
+      </c>
+      <c r="D23" s="0">
+        <v>0.15827428145937553</v>
+      </c>
+      <c r="E23" s="0">
+        <v>0.6220111471994294</v>
+      </c>
+      <c r="F23" s="0">
+        <v>0.11830239468631856</v>
+      </c>
+      <c r="G23" s="0">
+        <v>0.0017787522764088418</v>
+      </c>
+      <c r="H23" s="0">
+        <v>0.015035640496756156</v>
+      </c>
+      <c r="I23" s="0">
+        <v>0.015035640496756156</v>
+      </c>
+      <c r="J23" s="0">
+        <v>0.1030272487236889</v>
+      </c>
+      <c r="K23" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0.50860700529736635</v>
+      </c>
+      <c r="C24" s="0">
+        <v>0.60985728567059749</v>
+      </c>
+      <c r="D24" s="0">
+        <v>0.37798885296105333</v>
+      </c>
+      <c r="E24" s="0">
+        <v>0.84172571838014165</v>
+      </c>
+      <c r="F24" s="0">
+        <v>0.11830239460443806</v>
+      </c>
+      <c r="G24" s="0">
+        <v>0.0017787523440540851</v>
+      </c>
+      <c r="H24" s="0">
+        <v>0.0150356410789622</v>
+      </c>
+      <c r="I24" s="0">
+        <v>0.0150356410789622</v>
+      </c>
+      <c r="J24" s="0">
+        <v>0.10302724872368894</v>
+      </c>
+      <c r="K24" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" t="s">
+        <v>193</v>
+      </c>
+      <c r="G28" t="s">
+        <v>194</v>
+      </c>
+      <c r="H28" t="s">
+        <v>195</v>
+      </c>
+      <c r="I28" t="s">
+        <v>196</v>
+      </c>
+      <c r="J28" t="s">
+        <v>197</v>
+      </c>
+      <c r="K28" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>199</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0.53452888450843739</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0.61165685329914998</v>
+      </c>
+      <c r="D29" s="0">
+        <v>0.17582289468608406</v>
+      </c>
+      <c r="E29" s="0">
+        <v>1.0474908119122157</v>
+      </c>
+      <c r="F29" s="0">
+        <v>0.22236835066912897</v>
+      </c>
+      <c r="G29" s="0">
+        <v>0.01393725596215974</v>
+      </c>
+      <c r="H29" s="0">
+        <v>0.062676437182814557</v>
+      </c>
+      <c r="I29" s="0">
+        <v>0.062676437182814557</v>
+      </c>
+      <c r="J29" s="0">
+        <v>0.098516366541463785</v>
+      </c>
+      <c r="K29" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>200</v>
+      </c>
+      <c r="B30" s="0">
+        <v>-0.0053851758744829503</v>
+      </c>
+      <c r="C30" s="0">
+        <v>-0.28363375249536382</v>
+      </c>
+      <c r="D30" s="0">
+        <v>-0.91114256184009346</v>
+      </c>
+      <c r="E30" s="0">
+        <v>0.34387505684936581</v>
+      </c>
+      <c r="F30" s="0">
+        <v>0.32016343886644816</v>
+      </c>
+      <c r="G30" s="0">
+        <v>0.030253108311141499</v>
+      </c>
+      <c r="H30" s="0">
+        <v>0.094492701659670678</v>
+      </c>
+      <c r="I30" s="0">
+        <v>0.094492701659670678</v>
+      </c>
+      <c r="J30" s="0">
+        <v>0.31853731615374709</v>
+      </c>
+      <c r="K30" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="0">
+        <v>-0.52914370863395443</v>
+      </c>
+      <c r="C31" s="0">
+        <v>-0.32802310080378605</v>
+      </c>
+      <c r="D31" s="0">
+        <v>-0.87847023830571236</v>
+      </c>
+      <c r="E31" s="0">
+        <v>0.2224240366981402</v>
+      </c>
+      <c r="F31" s="0">
+        <v>0.28084553687913821</v>
+      </c>
+      <c r="G31" s="0">
+        <v>0.029768115449742335</v>
+      </c>
+      <c r="H31" s="0">
+        <v>0.10599461818242471</v>
+      </c>
+      <c r="I31" s="0">
+        <v>0.10599461818242471</v>
+      </c>
+      <c r="J31" s="0">
+        <v>0.22190530048377166</v>
+      </c>
+      <c r="K31" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" s="0">
+        <v>-4.5253302270781528e-15</v>
+      </c>
+      <c r="C32" s="0">
+        <v>-3.5239319302346658e-13</v>
+      </c>
+      <c r="D32" s="0">
+        <v>-1.0995990710866004e-11</v>
+      </c>
+      <c r="E32" s="0">
+        <v>1.0291204324819071e-11</v>
+      </c>
+      <c r="F32" s="0">
+        <v>5.4305066836931086e-12</v>
+      </c>
+      <c r="G32" s="0">
+        <v>1.1225254384841388e-12</v>
+      </c>
+      <c r="H32" s="0">
+        <v>0.20670731183425159</v>
+      </c>
+      <c r="I32" s="0">
+        <v>0.20670731183425159</v>
+      </c>
+      <c r="J32" s="0">
+        <v>3.7278295569788652e-13</v>
+      </c>
+      <c r="K32" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="0">
+        <v>-0.35873501092252547</v>
+      </c>
+      <c r="C33" s="0">
+        <v>-0.29420221881195269</v>
+      </c>
+      <c r="D33" s="0">
+        <v>-0.61957323529194808</v>
+      </c>
+      <c r="E33" s="0">
+        <v>0.031168797668042633</v>
+      </c>
+      <c r="F33" s="0">
+        <v>0.16600867110134701</v>
+      </c>
+      <c r="G33" s="0">
+        <v>0.049534897823508311</v>
+      </c>
+      <c r="H33" s="0">
+        <v>0.29838741250610723</v>
+      </c>
+      <c r="I33" s="0">
+        <v>0.29838741250610723</v>
+      </c>
+      <c r="J33" s="0">
+        <v>0.071057341958787198</v>
+      </c>
+      <c r="K33" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" s="0">
+        <v>0.35873501092253002</v>
+      </c>
+      <c r="C34" s="0">
+        <v>0.29420221881230507</v>
+      </c>
+      <c r="D34" s="0">
+        <v>-0.031168797600524573</v>
+      </c>
+      <c r="E34" s="0">
+        <v>0.61957323522513474</v>
+      </c>
+      <c r="F34" s="0">
+        <v>0.16600867106707817</v>
+      </c>
+      <c r="G34" s="0">
+        <v>0.049534897800557094</v>
+      </c>
+      <c r="H34" s="0">
+        <v>0.29838741242944961</v>
+      </c>
+      <c r="I34" s="0">
+        <v>0.29838741242944961</v>
+      </c>
+      <c r="J34" s="0">
+        <v>0.071057341958527406</v>
+      </c>
+      <c r="K34" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" s="0">
+        <v>-2.2626651135390764e-15</v>
+      </c>
+      <c r="C35" s="0">
+        <v>-1.6698456474634105e-13</v>
+      </c>
+      <c r="D35" s="0">
+        <v>-5.1809124542047919e-12</v>
+      </c>
+      <c r="E35" s="0">
+        <v>4.8469433247121091e-12</v>
+      </c>
+      <c r="F35" s="0">
+        <v>2.5581734812515308e-12</v>
+      </c>
+      <c r="G35" s="0">
+        <v>5.8673350962629082e-13</v>
+      </c>
+      <c r="H35" s="0">
+        <v>0.22935641930712386</v>
+      </c>
+      <c r="I35" s="0">
+        <v>0.22935641930712386</v>
+      </c>
+      <c r="J35" s="0">
+        <v>1.7777337971269686e-13</v>
+      </c>
+      <c r="K35" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="0">
+        <v>-0.17936750546126273</v>
+      </c>
+      <c r="C36" s="0">
+        <v>-0.13849399394658732</v>
+      </c>
+      <c r="D36" s="0">
+        <v>-0.29994295319468273</v>
+      </c>
+      <c r="E36" s="0">
+        <v>0.02295496530150809</v>
+      </c>
+      <c r="F36" s="0">
+        <v>0.082373431614858356</v>
+      </c>
+      <c r="G36" s="0">
+        <v>0.026137110720819298</v>
+      </c>
+      <c r="H36" s="0">
+        <v>0.31730025335140633</v>
+      </c>
+      <c r="I36" s="0">
+        <v>0.31730025335140633</v>
+      </c>
+      <c r="J36" s="0">
+        <v>0.044364599024101371</v>
+      </c>
+      <c r="K36" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="0">
+        <v>0.17936750546126501</v>
+      </c>
+      <c r="C37" s="0">
+        <v>0.13849399394675432</v>
+      </c>
+      <c r="D37" s="0">
+        <v>-0.022954965669756598</v>
+      </c>
+      <c r="E37" s="0">
+        <v>0.29994295356326528</v>
+      </c>
+      <c r="F37" s="0">
+        <v>0.082373431802828911</v>
+      </c>
+      <c r="G37" s="0">
+        <v>0.026137110933428624</v>
+      </c>
+      <c r="H37" s="0">
+        <v>0.31730025520839122</v>
+      </c>
+      <c r="I37" s="0">
+        <v>0.31730025520839122</v>
+      </c>
+      <c r="J37" s="0">
+        <v>0.044364599023975618</v>
+      </c>
+      <c r="K37" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="0">
+        <v>-0.18417155354769044</v>
+      </c>
+      <c r="C38" s="0">
+        <v>-0.27800868717520277</v>
+      </c>
+      <c r="D38" s="0">
+        <v>-0.46296786557083358</v>
+      </c>
+      <c r="E38" s="0">
+        <v>-0.093049508779571993</v>
+      </c>
+      <c r="F38" s="0">
+        <v>0.094368661799178577</v>
+      </c>
+      <c r="G38" s="0">
+        <v>0.027310280657375997</v>
+      </c>
+      <c r="H38" s="0">
+        <v>0.28939989331939131</v>
+      </c>
+      <c r="I38" s="0">
+        <v>0.28939989331939131</v>
+      </c>
+      <c r="J38" s="0">
+        <v>0.10918088361686869</v>
+      </c>
+      <c r="K38" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>209</v>
+      </c>
+      <c r="B39" s="0">
+        <v>0.18417155354769033</v>
+      </c>
+      <c r="C39" s="0">
+        <v>0.27800868717520277</v>
+      </c>
+      <c r="D39" s="0">
+        <v>0.093049508779571993</v>
+      </c>
+      <c r="E39" s="0">
+        <v>0.46296786557083358</v>
+      </c>
+      <c r="F39" s="0">
+        <v>0.094368661799178577</v>
+      </c>
+      <c r="G39" s="0">
+        <v>0.027310280657375997</v>
+      </c>
+      <c r="H39" s="0">
+        <v>0.28939989331939131</v>
+      </c>
+      <c r="I39" s="0">
+        <v>0.28939989331939131</v>
+      </c>
+      <c r="J39" s="0">
+        <v>0.10918088361686878</v>
+      </c>
+      <c r="K39" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>210</v>
+      </c>
+      <c r="B40" s="0">
+        <v>1.142046133388892e-16</v>
+      </c>
+      <c r="C40" s="0">
+        <v>4.4151415997608071e-18</v>
+      </c>
+      <c r="D40" s="0">
+        <v>-1.454347951899156e-16</v>
+      </c>
+      <c r="E40" s="0">
+        <v>1.5426507838943721e-16</v>
+      </c>
+      <c r="F40" s="0">
+        <v>7.6455454269401705e-17</v>
+      </c>
+      <c r="G40" s="0">
+        <v>6.6573622366394219e-17</v>
+      </c>
+      <c r="H40" s="0">
+        <v>0.8707504651246013</v>
+      </c>
+      <c r="I40" s="0">
+        <v>0.8707504651246013</v>
+      </c>
+      <c r="J40" s="0">
+        <v>1.0987821249047877e-16</v>
+      </c>
+      <c r="K40" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" s="0">
+        <v>0.36834310709538087</v>
+      </c>
+      <c r="C41" s="0">
+        <v>0.53352675070691258</v>
+      </c>
+      <c r="D41" s="0">
+        <v>0.1976388733567804</v>
+      </c>
+      <c r="E41" s="0">
+        <v>0.86941462805704472</v>
+      </c>
+      <c r="F41" s="0">
+        <v>0.1713745150418951</v>
+      </c>
+      <c r="G41" s="0">
+        <v>0.03538979099640506</v>
+      </c>
+      <c r="H41" s="0">
+        <v>0.20650556465617709</v>
+      </c>
+      <c r="I41" s="0">
+        <v>0.20650556465617709</v>
+      </c>
+      <c r="J41" s="0">
+        <v>0.1813052456166325</v>
+      </c>
+      <c r="K41" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" s="0">
+        <v>-0.36834310709538065</v>
+      </c>
+      <c r="C42" s="0">
+        <v>-0.53352675070691258</v>
+      </c>
+      <c r="D42" s="0">
+        <v>-0.86941462805704472</v>
+      </c>
+      <c r="E42" s="0">
+        <v>-0.1976388733567804</v>
+      </c>
+      <c r="F42" s="0">
+        <v>0.1713745150418951</v>
+      </c>
+      <c r="G42" s="0">
+        <v>0.03538979099640506</v>
+      </c>
+      <c r="H42" s="0">
+        <v>0.20650556465617709</v>
+      </c>
+      <c r="I42" s="0">
+        <v>0.20650556465617709</v>
+      </c>
+      <c r="J42" s="0">
+        <v>0.18130524561663275</v>
+      </c>
+      <c r="K42" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="0">
+        <v>-2.284092266777784e-16</v>
+      </c>
+      <c r="C43" s="0">
+        <v>-9.1163292786210058e-18</v>
+      </c>
+      <c r="D43" s="0">
+        <v>-3.0087638378620648e-16</v>
+      </c>
+      <c r="E43" s="0">
+        <v>2.8264372522896452e-16</v>
+      </c>
+      <c r="F43" s="0">
+        <v>1.4885990600284072e-16</v>
+      </c>
+      <c r="G43" s="0">
+        <v>1.4635811821655043e-16</v>
+      </c>
+      <c r="H43" s="0">
+        <v>0.9831936761652762</v>
+      </c>
+      <c r="I43" s="0">
+        <v>0.9831936761652762</v>
+      </c>
+      <c r="J43" s="0">
+        <v>2.1948230523036126e-16</v>
+      </c>
+      <c r="K43" s="0">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>